<commit_message>
Team Drive Backup Uploaded
</commit_message>
<xml_diff>
--- a/Deliverable Submissions/Team Google Drive Backup/Team Drive/THE PROJECT/Product Backlog.xlsx
+++ b/Deliverable Submissions/Team Google Drive Backup/Team Drive/THE PROJECT/Product Backlog.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="Deliverable 1 Sprint" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Deliverable 2 Sprint" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Deliverable 3 Sprint" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="83">
   <si>
     <t>Deliverable 1</t>
   </si>
@@ -73,12 +74,12 @@
     <t>User Story</t>
   </si>
   <si>
-    <t>Story Tasks</t>
-  </si>
-  <si>
     <t>Sprint Number</t>
   </si>
   <si>
+    <t>Story Points</t>
+  </si>
+  <si>
     <t>Sprint Goal</t>
   </si>
   <si>
@@ -89,9 +90,6 @@
   </si>
   <si>
     <t>Story Status</t>
-  </si>
-  <si>
-    <t>Story Points</t>
   </si>
   <si>
     <t>Story Points Completed</t>
@@ -292,13 +290,34 @@
   </si>
   <si>
     <t>Deliverable 2</t>
+  </si>
+  <si>
+    <t>Deliverable 3</t>
+  </si>
+  <si>
+    <t>Names Of Contributors</t>
+  </si>
+  <si>
+    <t>Contribution Percentages</t>
+  </si>
+  <si>
+    <t>In-progress</t>
+  </si>
+  <si>
+    <t>Kevin Menello</t>
+  </si>
+  <si>
+    <t>Samson Cournane</t>
+  </si>
+  <si>
+    <t>Unassigned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -315,13 +334,6 @@
       <b/>
       <sz val="12.0"/>
       <color theme="1"/>
-      <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12.0"/>
-      <color rgb="FF0000FF"/>
       <name val="Trebuchet MS"/>
     </font>
     <font>
@@ -383,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -399,54 +411,72 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,6 +491,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -678,7 +712,7 @@
     <col customWidth="1" min="4" max="4" width="14.63"/>
     <col customWidth="1" min="5" max="5" width="12.25"/>
     <col customWidth="1" min="6" max="6" width="15.5"/>
-    <col customWidth="1" min="7" max="12" width="21.88"/>
+    <col customWidth="1" min="7" max="11" width="21.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">
@@ -696,7 +730,7 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -714,305 +748,291 @@
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="11">
         <v>8.0</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="11">
         <v>8.0</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="11">
         <v>10.0</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="C7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="11">
         <v>5.0</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="11">
         <v>8.0</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>36</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="11">
         <v>8.0</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="D10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="11">
         <v>10.0</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="11">
         <v>10.0</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="D12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="11">
         <v>4.0</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="D13" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="11">
         <v>5.0</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="17"/>
@@ -1026,101 +1046,96 @@
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="C16" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>52</v>
-      </c>
       <c r="D16" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="11">
         <v>7.0</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="11">
         <v>8.0</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="D18" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="11">
         <v>6.0</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="17"/>
@@ -1134,77 +1149,73 @@
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>62</v>
-      </c>
       <c r="D21" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="11">
         <v>8.0</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="D22" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="11">
         <v>5.0</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -1216,101 +1227,97 @@
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="D24" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="11">
         <v>7.0</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="11">
         <v>9.0</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="D26" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" s="11">
         <v>6.0</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A20:G20"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:K13 G16:K18 G21:K22 G24:K26">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:J13 G16:J18 G21:J22 G24:J26">
       <formula1>"Unassigned,Waiting,In-progress,Testing,Done"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F13 F16:F18 F21:F22 F24:F26">
@@ -1321,15 +1328,13 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="E2"/>
-    <hyperlink r:id="rId3" ref="G2"/>
-    <hyperlink r:id="rId4" ref="J2"/>
+    <hyperlink r:id="rId2" ref="G2"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1353,13 +1358,13 @@
     <col customWidth="1" min="4" max="4" width="14.63"/>
     <col customWidth="1" min="5" max="5" width="12.25"/>
     <col customWidth="1" min="6" max="6" width="15.5"/>
-    <col customWidth="1" min="7" max="11" width="21.88"/>
-    <col customWidth="1" min="12" max="12" width="34.75"/>
+    <col customWidth="1" min="7" max="10" width="21.88"/>
+    <col customWidth="1" min="11" max="11" width="34.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="39.75" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" ht="21.75" customHeight="1">
@@ -1372,7 +1377,7 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1384,311 +1389,317 @@
       <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="22" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="H3" s="23"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="11">
         <v>8.0</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="11">
         <v>8.0</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="11">
         <v>10.0</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="C7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="11">
         <v>5.0</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="11">
         <v>8.0</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>36</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="11">
         <v>8.0</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="D10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="11">
         <v>10.0</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="11">
         <v>10.0</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="D12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="11">
         <v>4.0</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="D13" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="11">
         <v>5.0</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="17"/>
@@ -1698,105 +1709,106 @@
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="19"/>
+        <v>48</v>
+      </c>
+      <c r="H15" s="25"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="C16" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>52</v>
-      </c>
       <c r="D16" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="11">
         <v>7.0</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="11">
         <v>8.0</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="D18" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="11">
         <v>6.0</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="17"/>
@@ -1806,81 +1818,81 @@
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="19"/>
+        <v>58</v>
+      </c>
+      <c r="H20" s="25"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>62</v>
-      </c>
       <c r="D21" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="11">
         <v>8.0</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="D22" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="11">
         <v>5.0</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -1888,108 +1900,110 @@
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="H23" s="26"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="D24" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="11">
         <v>7.0</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="11">
         <v>9.0</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="D26" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" s="11">
         <v>6.0</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A20:G20"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:K13 G16:K18 G21:K22 G24:K26">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G13 I4:J13 G16:G18 I16:J18 G21:G22 I21:J22 G24:G26 I24:J26">
       <formula1>"Unassigned,Waiting,In-progress,Testing,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F13 F16:F18 F21:F22 F24:F26">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F13 H4:H13 F16:F18 H16:H18 F21:F22 H21:H22 F24:F26 H24:H26">
       <formula1>"Unassigned,Low,Medium,High"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4:E13 E16:E18 E21:E22 E24:E26">
@@ -1997,13 +2011,823 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
-    <hyperlink r:id="rId2" ref="G2"/>
-    <hyperlink r:id="rId3" ref="J2"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.0"/>
+    <col customWidth="1" min="2" max="2" width="48.13"/>
+    <col customWidth="1" min="3" max="3" width="51.75"/>
+    <col customWidth="1" min="4" max="5" width="14.63"/>
+    <col customWidth="1" min="6" max="6" width="15.5"/>
+    <col customWidth="1" min="7" max="10" width="21.88"/>
+    <col customWidth="1" min="11" max="12" width="34.75"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="39.75" customHeight="1">
+      <c r="A1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" ht="21.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="27">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="25"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="11">
+        <v>6.0</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="25"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="11">
+        <v>9.0</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="11">
+        <v>6.0</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A21:G21"/>
+  </mergeCells>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4 I4 G6:G14 I6:I14 G17:G19 I17:I19 G22:G23 I22:I23 G25:G27 I25:I27">
+      <formula1>"Unassigned,Waiting,In-progress,Testing,Done"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4 H4 F6:F14 H6:H14 F17:F19 H17:H19 F22:F23 H22:H23 F25:F27 H25:H27">
+      <formula1>"Unassigned,Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4 E6:E14 E17:E19 E22:E23 E25:E27">
+      <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L4:L5">
+      <formula1>"10%,20%,30%,40%,50%,60%,70%,80%,90%,100%"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J4 J6:J14 J17:J19 J22:J23 J25:J27">
+      <formula1>"Unassigned,1,2,3,4,5,6,7,8,9,10"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K5">
+      <formula1>"Kevin Menello,Samson Cournane,Sam Minor,Andrew Bement,Emily Brule,Tereza Holubcova"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G2"/>
+  </hyperlinks>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>